<commit_message>
Table for prediction(in jin.tex)
</commit_message>
<xml_diff>
--- a/paper/figures/predictionPerformance.xlsx
+++ b/paper/figures/predictionPerformance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\mmprof\paper\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F421CC43-E0F6-496B-BDD9-F32F7516611F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE42E3A2-E653-4A08-B4DF-E88F933D332A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4905" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>benchmark</t>
   </si>
@@ -48,51 +49,55 @@
     <t>swaptions</t>
   </si>
   <si>
-    <t>Default-truth</t>
+    <t>Dieharder-real</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>glibc-2.21-truth</t>
+    <t>Dieharder-predict</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>jemalloc-truth</t>
+    <t>Default-real</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>TcMalloc-truth</t>
+    <t>Default-predict</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Hoard-truth</t>
+    <t>glibc-2.21-real</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Default-prediction</t>
+    <t>glibc-2.21-predict</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>glibc-2.21-prediction</t>
+    <t>jemalloc-real</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>jemalloc-prediction</t>
+    <t>jemalloc-predict</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>TcMalloc-prediction</t>
+    <t>TcMalloc-real</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Hoard-prediction</t>
+    <t>TcMalloc-predict</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>real</t>
+    <t>Hoard-predict</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>predict</t>
+    <t>Hoard-real</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>freqmine</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -181,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -208,6 +213,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -265,31 +273,33 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Default-truth</c:v>
+                  <c:v>Default-real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="pct5">
+            <a:pattFill prst="wdDnDiag">
               <a:fgClr>
-                <a:schemeClr val="bg1"/>
+                <a:schemeClr val="tx1"/>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="bg1"/>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -297,15 +307,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -313,10 +326,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.05</c:v>
                 </c:pt>
@@ -324,15 +337,18 @@
                   <c:v>1.06</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.1599999999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.27</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.99</c:v>
                 </c:pt>
               </c:numCache>
@@ -353,31 +369,33 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Default-prediction</c:v>
+                  <c:v>Default-predict</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="pct10">
+            <a:pattFill prst="wdUpDiag">
               <a:fgClr>
-                <a:schemeClr val="bg1"/>
+                <a:schemeClr val="tx1"/>
               </a:fgClr>
               <a:bgClr>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="bg1"/>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -385,15 +403,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -401,10 +422,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.05</c:v>
                 </c:pt>
@@ -415,12 +436,15 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.02</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.07</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.99</c:v>
                 </c:pt>
               </c:numCache>
@@ -441,7 +465,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>glibc-2.21-truth</c:v>
+                  <c:v>glibc-2.21-real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -456,16 +480,18 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -473,15 +499,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -489,10 +518,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.07</c:v>
                 </c:pt>
@@ -500,15 +529,18 @@
                   <c:v>1.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.1599999999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.27</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.99</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.99</c:v>
                 </c:pt>
               </c:numCache>
@@ -529,7 +561,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>glibc-2.21-prediction</c:v>
+                  <c:v>glibc-2.21-predict</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -544,16 +576,18 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -561,15 +595,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -577,10 +614,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:f>Sheet1!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.06</c:v>
                 </c:pt>
@@ -591,12 +628,15 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.05</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.07</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -617,7 +657,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>jemalloc-truth</c:v>
+                  <c:v>jemalloc-real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -632,16 +672,18 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -649,15 +691,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -665,10 +710,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:f>Sheet1!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.01</c:v>
                 </c:pt>
@@ -676,15 +721,18 @@
                   <c:v>1.06</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.06</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.05</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.98</c:v>
                 </c:pt>
               </c:numCache>
@@ -705,7 +753,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>jemalloc-prediction</c:v>
+                  <c:v>jemalloc-predict</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -720,16 +768,18 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -737,15 +787,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -753,10 +806,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$7</c:f>
+              <c:f>Sheet1!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.03</c:v>
                 </c:pt>
@@ -770,9 +823,12 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.08</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.96</c:v>
                 </c:pt>
               </c:numCache>
@@ -793,7 +849,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TcMalloc-truth</c:v>
+                  <c:v>TcMalloc-real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -808,16 +864,18 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -825,15 +883,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -841,10 +902,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$7</c:f>
+              <c:f>Sheet1!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -861,6 +922,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -881,7 +945,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TcMalloc-prediction</c:v>
+                  <c:v>TcMalloc-predict</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -896,16 +960,18 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -913,15 +979,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -929,10 +998,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$7</c:f>
+              <c:f>Sheet1!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.02</c:v>
                 </c:pt>
@@ -946,9 +1015,12 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.04</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.96</c:v>
                 </c:pt>
               </c:numCache>
@@ -969,7 +1041,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hoard-truth</c:v>
+                  <c:v>Hoard-real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -984,16 +1056,18 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -1001,15 +1075,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -1017,10 +1094,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$7</c:f>
+              <c:f>Sheet1!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.03</c:v>
                 </c:pt>
@@ -1028,15 +1105,18 @@
                   <c:v>1.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.02</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.1499999999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -1057,7 +1137,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hoard-prediction</c:v>
+                  <c:v>Hoard-predict</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1072,16 +1152,18 @@
               </a:bgClr>
             </a:pattFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>canneal</c:v>
                 </c:pt>
@@ -1089,15 +1171,18 @@
                   <c:v>dedup</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>kmeans</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>raytrace</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>reverse_index</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>swaptions</c:v>
                 </c:pt>
               </c:strCache>
@@ -1105,10 +1190,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$7</c:f>
+              <c:f>Sheet1!$K$2:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.1100000000000001</c:v>
                 </c:pt>
@@ -1119,12 +1204,15 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.01</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.1599999999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.1100000000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -1133,6 +1221,202 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000F-714D-44C3-B8D5-BF3119E04945}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dieharder-real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dashDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DDEB-4314-954E-321A8C3E5AB2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dieharder-predict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dashUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.51</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DDEB-4314-954E-321A8C3E5AB2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1203,8 +1487,8 @@
         <c:axId val="407555904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.1500000000000001"/>
-          <c:min val="0.95000000000000007"/>
+          <c:max val="1.5"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1322,7 +1606,7 @@
         <c:crossAx val="277828176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="5.000000000000001E-2"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1338,10 +1622,1472 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.1013240750025551E-2"/>
-          <c:y val="0.1352440107947418"/>
-          <c:w val="0.95920320675597637"/>
-          <c:h val="0.13705528744390821"/>
+          <c:x val="1.979444448496346E-2"/>
+          <c:y val="9.4566128386494058E-2"/>
+          <c:w val="0.97898678623784929"/>
+          <c:h val="0.16639174340495574"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.185740827940886E-2"/>
+          <c:y val="0.31780821917808222"/>
+          <c:w val="0.9234649618594617"/>
+          <c:h val="0.40855168910337819"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Default-real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Default-predict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>glibc-2.21-real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>glibc-2.21-predict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>jemalloc-real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dashDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>jemalloc-predict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dashUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TcMalloc-real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$H$2:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TcMalloc-predict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hoard-real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$J$2:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hoard-predict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="bg1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="tx1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$K$2:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dieharder-real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dashDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$L$2:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dieharder-predict</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dashUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="tx1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>freqmine</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.51</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-D584-4872-AF20-56F1D2F05B3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="199"/>
+        <c:axId val="277828176"/>
+        <c:axId val="407555904"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="277828176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="407555904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="407555904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.4"/>
+          <c:min val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" cap="none" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Normalized Runtime</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.9788785035407603E-3"/>
+              <c:y val="0.28121577346168986"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="277828176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.979444448496346E-2"/>
+          <c:y val="9.4566128386494058E-2"/>
+          <c:w val="0.97898678623784929"/>
+          <c:h val="0.16639174340495574"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1451,6 +3197,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
   <cs:axisTitle>
@@ -1951,20 +3737,520 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>828676</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>876301</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>566737</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>885824</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1993,6 +4279,175 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.06822</cdr:x>
+      <cdr:y>0.24871</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96749</cdr:x>
+      <cdr:y>0.31732</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9B62555-920E-41F8-8C54-92F3B531FFC0}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="709612" y="690563"/>
+          <a:ext cx="9353550" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.05393</cdr:x>
+      <cdr:y>0.247</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.98031</cdr:x>
+      <cdr:y>0.34648</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2194C8EF-D8AD-45BE-8982-2FD27601C8AB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="561974" y="694039"/>
+          <a:ext cx="9653197" cy="279526"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>                                  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>  2.0</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>                                  2.9</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> 1.9</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>                                  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>3.3    </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>876301</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>885824</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41931F1B-60E5-40A8-9274-1F2157C0A86B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -2360,10 +4815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2379,44 +4834,52 @@
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="12.796875" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14.9296875" customWidth="1"/>
+    <col min="13" max="13" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="37.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="37.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2450,8 +4913,14 @@
       <c r="K2" s="8">
         <v>1.1100000000000001</v>
       </c>
+      <c r="L2" s="10">
+        <v>1.39</v>
+      </c>
+      <c r="M2" s="10">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -2485,25 +4954,31 @@
       <c r="K3" s="8">
         <v>1</v>
       </c>
+      <c r="L3" s="10">
+        <v>2.91</v>
+      </c>
+      <c r="M3" s="10">
+        <v>1.89</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7">
-        <v>1.1599999999999999</v>
+        <v>0.9</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
       </c>
       <c r="D4" s="7">
-        <v>1.1599999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="E4" s="8">
         <v>1</v>
       </c>
       <c r="F4" s="8">
-        <v>1.06</v>
+        <v>1.01</v>
       </c>
       <c r="G4" s="8">
         <v>1</v>
@@ -2515,30 +4990,36 @@
         <v>1</v>
       </c>
       <c r="J4" s="8">
-        <v>1.02</v>
+        <v>1.26</v>
       </c>
       <c r="K4" s="8">
         <v>1</v>
       </c>
+      <c r="L4" s="10">
+        <v>3.32</v>
+      </c>
+      <c r="M4" s="10">
+        <v>1.01</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>1.27</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C5" s="8">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="D5" s="7">
-        <v>1.27</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E5" s="8">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="F5" s="8">
-        <v>1.2</v>
+        <v>1.06</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
@@ -2550,131 +5031,178 @@
         <v>1</v>
       </c>
       <c r="J5" s="8">
-        <v>1.1000000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="K5" s="8">
-        <v>1.01</v>
+        <v>1</v>
+      </c>
+      <c r="L5" s="10">
+        <v>1.03</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="7">
+        <v>1.27</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.27</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1.05</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="8">
         <v>1</v>
-      </c>
-      <c r="C6" s="8">
-        <v>1.07</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.99</v>
-      </c>
-      <c r="E6" s="8">
-        <v>1.07</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1.05</v>
-      </c>
-      <c r="G6" s="8">
-        <v>1.08</v>
       </c>
       <c r="H6" s="8">
         <v>1</v>
       </c>
       <c r="I6" s="8">
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="J6" s="8">
-        <v>1.1499999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K6" s="8">
-        <v>1.1599999999999999</v>
+        <v>1.01</v>
+      </c>
+      <c r="L6" s="10">
+        <v>1.31</v>
+      </c>
+      <c r="M6" s="10">
+        <v>1.51</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="C7" s="8">
-        <v>0.99</v>
+        <v>1.07</v>
       </c>
       <c r="D7" s="7">
         <v>0.99</v>
       </c>
-      <c r="E7" s="7">
-        <v>1</v>
+      <c r="E7" s="8">
+        <v>1.07</v>
       </c>
       <c r="F7" s="8">
-        <v>0.98</v>
+        <v>1.05</v>
       </c>
       <c r="G7" s="8">
-        <v>0.96</v>
+        <v>1.08</v>
       </c>
       <c r="H7" s="8">
         <v>1</v>
       </c>
       <c r="I7" s="8">
+        <v>1.04</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="L7" s="10">
+        <v>2.42</v>
+      </c>
+      <c r="M7" s="10">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="G8" s="8">
         <v>0.96</v>
       </c>
-      <c r="J7" s="8">
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="J8" s="8">
         <v>2.04</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K8" s="8">
         <v>1.1100000000000001</v>
       </c>
+      <c r="L8" s="10">
+        <v>5.67</v>
+      </c>
+      <c r="M8" s="10">
+        <v>3.82</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="9"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="2"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="9"/>
-      <c r="C11" s="4"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="9"/>
       <c r="G11" s="4"/>
       <c r="H11" s="9"/>
       <c r="I11" s="4"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="9"/>
       <c r="C12" s="4"/>
@@ -2686,7 +5214,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
       <c r="B13" s="9"/>
       <c r="C13" s="4"/>
@@ -2698,7 +5226,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="9"/>
       <c r="C14" s="4"/>
@@ -2710,11 +5238,11 @@
       <c r="I14" s="4"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
       <c r="B15" s="9"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="4"/>
       <c r="F15" s="9"/>
       <c r="G15" s="4"/>
@@ -2722,16 +5250,16 @@
       <c r="I15" s="4"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
@@ -2770,13 +5298,522 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="C27" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0B0CB7-D6FF-45EF-AE95-0D14E70A71D4}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="16.46484375" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" customWidth="1"/>
+    <col min="3" max="3" width="18.1328125" customWidth="1"/>
+    <col min="4" max="4" width="15.265625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" customWidth="1"/>
+    <col min="8" max="8" width="14.3984375" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="12.796875" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14.9296875" customWidth="1"/>
+    <col min="13" max="13" width="17.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="37.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D27" t="s">
-        <v>18</v>
-      </c>
+      <c r="L1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1.01</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1.03</v>
+      </c>
+      <c r="K2" s="8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="L2" s="10">
+        <v>1.39</v>
+      </c>
+      <c r="M2" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.01</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1.35</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1.01</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10">
+        <v>2.91</v>
+      </c>
+      <c r="M3" s="10">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.96</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1.01</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8">
+        <v>1.26</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10">
+        <v>3.32</v>
+      </c>
+      <c r="M4" s="10">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10">
+        <v>1.03</v>
+      </c>
+      <c r="M5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1.27</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1.02</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.27</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1.05</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1.01</v>
+      </c>
+      <c r="L6" s="10">
+        <v>1.31</v>
+      </c>
+      <c r="M6" s="10">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1.05</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1.08</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1.04</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="L7" s="10">
+        <v>2.42</v>
+      </c>
+      <c r="M7" s="10">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="J8" s="8">
+        <v>2.04</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="L8" s="10">
+        <v>5.67</v>
+      </c>
+      <c r="M8" s="10">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
a figure for mmprof overhead
</commit_message>
<xml_diff>
--- a/paper/figures/predictionPerformance.xlsx
+++ b/paper/figures/predictionPerformance.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\mmprof\paper\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE42E3A2-E653-4A08-B4DF-E88F933D332A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5983EB1-BD9B-4CA3-906D-9AEB57E542C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4905" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="table" sheetId="3" r:id="rId1"/>
+    <sheet name="figure" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="37">
   <si>
     <t>benchmark</t>
   </si>
@@ -100,12 +100,85 @@
     <t>freqmine</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>Applications</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>canneal</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>dedup</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>freqmine</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>kmeans</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>raytrace</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>reverse_index</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>swaptions</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prediction</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Allocator</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>glibc-2.21</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>jemalloc</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TcMalloc</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hoard</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dieharder</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="0.00_ "/>
+    <numFmt numFmtId="182" formatCode="0.0_ "/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +215,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -183,10 +263,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -216,8 +299,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="182" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -269,7 +388,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>figure!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -297,7 +416,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -326,7 +445,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>figure!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -365,7 +484,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>figure!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -393,7 +512,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -422,7 +541,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>figure!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -461,7 +580,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>figure!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -489,7 +608,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -518,7 +637,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>figure!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -557,7 +676,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>figure!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -585,7 +704,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -614,7 +733,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:f>figure!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -653,7 +772,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>figure!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -681,7 +800,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -710,7 +829,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$8</c:f>
+              <c:f>figure!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -749,7 +868,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>figure!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -777,7 +896,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -806,7 +925,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$8</c:f>
+              <c:f>figure!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -845,7 +964,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>figure!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -873,7 +992,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -902,7 +1021,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$8</c:f>
+              <c:f>figure!$H$2:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -941,7 +1060,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>figure!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -969,7 +1088,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -998,7 +1117,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$8</c:f>
+              <c:f>figure!$I$2:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1037,7 +1156,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>figure!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1065,7 +1184,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1094,7 +1213,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$8</c:f>
+              <c:f>figure!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1133,7 +1252,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>figure!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1161,7 +1280,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1190,7 +1309,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$8</c:f>
+              <c:f>figure!$K$2:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1229,7 +1348,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1</c:f>
+              <c:f>figure!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1259,7 +1378,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1288,7 +1407,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$8</c:f>
+              <c:f>figure!$L$2:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1327,7 +1446,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$1</c:f>
+              <c:f>figure!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1357,7 +1476,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>figure!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1386,7 +1505,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$8</c:f>
+              <c:f>figure!$M$2:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1695,1509 +1814,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.185740827940886E-2"/>
-          <c:y val="0.31780821917808222"/>
-          <c:w val="0.9234649618594617"/>
-          <c:h val="0.40855168910337819"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Default-real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="wdDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="tx1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$B$2:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.06</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1599999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.99</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Default-predict</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="wdUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="tx1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$C$2:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.05</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.02</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.07</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.99</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>glibc-2.21-real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="ltDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="tx1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$D$2:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.07</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1599999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.99</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.99</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>glibc-2.21-predict</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="ltUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="tx1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$E$2:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.06</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.05</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.07</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>jemalloc-real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="dashDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="tx1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$F$2:$F$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.06</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.06</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.05</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.98</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>jemalloc-predict</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="dashUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="tx1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$G$2:$G$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.03</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.08</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.96</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TcMalloc-real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="wdDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="tx1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$H$2:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TcMalloc-predict</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="wdUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="tx1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$I$2:$I$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.02</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.04</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.96</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$J$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Hoard-real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="dkDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="tx1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$J$2:$J$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.03</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.02</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.26</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.02</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.04</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$K$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Hoard-predict</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="dkUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="bg1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="tx1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$K$2:$K$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.1100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.01</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1599999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.1100000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$L$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Dieharder-real</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="dashDnDiag">
-              <a:fgClr>
-                <a:schemeClr val="tx1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="90000"/>
-                </a:schemeClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$L$2:$L$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.39</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.91</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.03</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.31</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.42</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.67</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Dieharder-predict</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:pattFill prst="dashUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="tx1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="90000"/>
-                </a:schemeClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Sheet1 (2)'!$A$2:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>canneal</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>dedup</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>freqmine</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>kmeans</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>raytrace</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>reverse_index</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>swaptions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sheet1 (2)'!$M$2:$M$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.89</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.51</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.89</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.82</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-D584-4872-AF20-56F1D2F05B3E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="199"/>
-        <c:axId val="277828176"/>
-        <c:axId val="407555904"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="277828176"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="407555904"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="407555904"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.4"/>
-          <c:min val="0.8"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" cap="none" baseline="0">
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
-                  <a:t>Normalized Runtime</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="8.9788785035407603E-3"/>
-              <c:y val="0.28121577346168986"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="zh-CN"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="277828176"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="0.1"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="1.979444448496346E-2"/>
-          <c:y val="9.4566128386494058E-2"/>
-          <c:w val="0.97898678623784929"/>
-          <c:h val="0.16639174340495574"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:userShapes r:id="rId3"/>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3737,520 +2354,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="38100" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>876301</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1133476</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>885824</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>866774</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4320,12 +2437,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.05393</cdr:x>
-      <cdr:y>0.247</cdr:y>
+      <cdr:x>0.0521</cdr:x>
+      <cdr:y>0.25039</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.98031</cdr:x>
-      <cdr:y>0.34648</cdr:y>
+      <cdr:x>0.99817</cdr:x>
+      <cdr:y>0.34987</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4340,8 +2457,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="561974" y="694039"/>
-          <a:ext cx="9653197" cy="279526"/>
+          <a:off x="542924" y="703564"/>
+          <a:ext cx="9858374" cy="279526"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4363,7 +2480,7 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>  2.0</a:t>
+            <a:t>   2.0</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
@@ -4384,162 +2501,14 @@
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>                                  </a:t>
+            <a:t>                                 </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0">
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>3.3    </a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
-            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>876301</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>885824</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41931F1B-60E5-40A8-9274-1F2157C0A86B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.06822</cdr:x>
-      <cdr:y>0.24871</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.96749</cdr:x>
-      <cdr:y>0.31732</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9B62555-920E-41F8-8C54-92F3B531FFC0}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="709612" y="690563"/>
-          <a:ext cx="9353550" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.23901</cdr:x>
-      <cdr:y>0.247</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.98031</cdr:x>
-      <cdr:y>0.34648</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2194C8EF-D8AD-45BE-8982-2FD27601C8AB}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2486024" y="685800"/>
-          <a:ext cx="7710488" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>1.35                                  1.16   1.16                                 1.27</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" baseline="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>   1.27   1.2                                                           1.15  1.16                                    2.04</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>                               </a:t>
+            <a:t>3.3                                                                                     1.5                                  2.4 1.9                           2.0 5.7 3.8  </a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -4814,11 +2783,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0B70CD-7B84-4635-A7BE-AF3CE3C3A248}">
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -5166,164 +3135,1012 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-    </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A14" s="2"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A15" s="2"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.4">
-      <c r="A16" s="2"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="A10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1.05</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1.05</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="20">
+        <v>1.05</v>
+      </c>
+      <c r="I11" s="20">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="13"/>
+      <c r="B12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1.07</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1.06</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="21">
+        <v>1.07</v>
+      </c>
+      <c r="I12" s="21">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="13"/>
+      <c r="B13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1.01</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1.03</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="22">
+        <v>1.01</v>
+      </c>
+      <c r="I13" s="22">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="13"/>
+      <c r="B14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="22">
+        <v>1</v>
+      </c>
+      <c r="I14" s="22">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="13"/>
+      <c r="B15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1.03</v>
+      </c>
+      <c r="D15" s="15">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="22">
+        <v>1.03</v>
+      </c>
+      <c r="I15" s="22">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="13"/>
+      <c r="B16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1.39</v>
+      </c>
+      <c r="D16" s="16">
+        <v>2</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="23">
+        <v>1.39</v>
+      </c>
+      <c r="I16" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1.06</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1.01</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="21">
+        <v>1.06</v>
+      </c>
+      <c r="I17" s="22">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="17"/>
+      <c r="B18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1.35</v>
+      </c>
+      <c r="D18" s="15">
+        <v>1.01</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="21">
+        <v>1.35</v>
+      </c>
+      <c r="I18" s="22">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="17"/>
+      <c r="B19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="15">
+        <v>1.06</v>
+      </c>
+      <c r="D19" s="15">
+        <v>1</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="22">
+        <v>1.06</v>
+      </c>
+      <c r="I19" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="17"/>
+      <c r="B20" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="15">
+        <v>1</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="22">
+        <v>1</v>
+      </c>
+      <c r="I20" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="17"/>
+      <c r="B21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="D21" s="15">
+        <v>1</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="22">
+        <v>1.02</v>
+      </c>
+      <c r="I21" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" s="17"/>
+      <c r="B22" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="16">
+        <v>2.91</v>
+      </c>
+      <c r="D22" s="16">
+        <v>1.89</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="23">
+        <v>2.91</v>
+      </c>
+      <c r="I22" s="23">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="D23" s="15">
+        <v>1</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="I23" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24" s="18"/>
+      <c r="B24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="14">
+        <v>0.96</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="21">
+        <v>0.96</v>
+      </c>
+      <c r="I24" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" s="18"/>
+      <c r="B25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1.01</v>
+      </c>
+      <c r="D25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="22">
+        <v>1.01</v>
+      </c>
+      <c r="I25" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26" s="18"/>
+      <c r="B26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="15">
+        <v>1</v>
+      </c>
+      <c r="D26" s="15">
+        <v>1</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="22">
+        <v>1</v>
+      </c>
+      <c r="I26" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27" s="18"/>
+      <c r="B27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="15">
+        <v>1.26</v>
+      </c>
+      <c r="D27" s="15">
+        <v>1</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="22">
+        <v>1.26</v>
+      </c>
+      <c r="I27" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A28" s="18"/>
+      <c r="B28" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="16">
+        <v>3.32</v>
+      </c>
+      <c r="D28" s="16">
+        <v>1.01</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="23">
+        <v>3.32</v>
+      </c>
+      <c r="I28" s="23">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A29" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D29" s="15">
+        <v>1</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="21">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="I29" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" s="18"/>
+      <c r="B30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="14">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D30" s="15">
+        <v>1</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="21">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="I30" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31" s="18"/>
+      <c r="B31" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="15">
+        <v>1.06</v>
+      </c>
+      <c r="D31" s="15">
+        <v>1</v>
+      </c>
+      <c r="F31" s="18"/>
+      <c r="G31" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="22">
+        <v>1.06</v>
+      </c>
+      <c r="I31" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" s="18"/>
+      <c r="B32" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="15">
+        <v>1</v>
+      </c>
+      <c r="D32" s="15">
+        <v>1</v>
+      </c>
+      <c r="F32" s="18"/>
+      <c r="G32" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="22">
+        <v>1</v>
+      </c>
+      <c r="I32" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="18"/>
+      <c r="B33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="D33" s="15">
+        <v>1</v>
+      </c>
+      <c r="F33" s="18"/>
+      <c r="G33" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="22">
+        <v>1.02</v>
+      </c>
+      <c r="I33" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="18"/>
+      <c r="B34" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="16">
+        <v>1.03</v>
+      </c>
+      <c r="D34" s="16">
+        <v>1</v>
+      </c>
+      <c r="F34" s="18"/>
+      <c r="G34" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" s="23">
+        <v>1.03</v>
+      </c>
+      <c r="I34" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A35" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="D35" s="15">
+        <v>1.02</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" s="21">
+        <v>1.27</v>
+      </c>
+      <c r="I35" s="22">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A36" s="19"/>
+      <c r="B36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="14">
+        <v>1.27</v>
+      </c>
+      <c r="D36" s="15">
+        <v>1.05</v>
+      </c>
+      <c r="F36" s="19"/>
+      <c r="G36" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="21">
+        <v>1.27</v>
+      </c>
+      <c r="I36" s="22">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="19"/>
+      <c r="B37" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="D37" s="15">
+        <v>1</v>
+      </c>
+      <c r="F37" s="19"/>
+      <c r="G37" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="I37" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="19"/>
+      <c r="B38" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="15">
+        <v>1</v>
+      </c>
+      <c r="D38" s="15">
+        <v>1</v>
+      </c>
+      <c r="F38" s="19"/>
+      <c r="G38" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="22">
+        <v>1</v>
+      </c>
+      <c r="I38" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A39" s="19"/>
+      <c r="B39" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D39" s="15">
+        <v>1.01</v>
+      </c>
+      <c r="F39" s="19"/>
+      <c r="G39" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I39" s="22">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A40" s="19"/>
+      <c r="B40" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="16">
+        <v>1.31</v>
+      </c>
+      <c r="D40" s="16">
+        <v>1.51</v>
+      </c>
+      <c r="F40" s="19"/>
+      <c r="G40" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H40" s="23">
+        <v>1.31</v>
+      </c>
+      <c r="I40" s="23">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="14">
+        <v>1</v>
+      </c>
+      <c r="D41" s="15">
+        <v>1.07</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="21">
+        <v>1</v>
+      </c>
+      <c r="I41" s="22">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A42" s="18"/>
+      <c r="B42" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="14">
+        <v>0.99</v>
+      </c>
+      <c r="D42" s="15">
+        <v>1.07</v>
+      </c>
+      <c r="F42" s="18"/>
+      <c r="G42" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="I42" s="22">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A43" s="18"/>
+      <c r="B43" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="15">
+        <v>1.05</v>
+      </c>
+      <c r="D43" s="15">
+        <v>1.08</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="22">
+        <v>1.05</v>
+      </c>
+      <c r="I43" s="22">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A44" s="18"/>
+      <c r="B44" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="15">
+        <v>1</v>
+      </c>
+      <c r="D44" s="15">
+        <v>1.04</v>
+      </c>
+      <c r="F44" s="18"/>
+      <c r="G44" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H44" s="22">
+        <v>1</v>
+      </c>
+      <c r="I44" s="22">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A45" s="18"/>
+      <c r="B45" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="15">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D45" s="15">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="G45" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="22">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I45" s="22">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="18"/>
+      <c r="B46" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="16">
+        <v>2.42</v>
+      </c>
+      <c r="D46" s="16">
+        <v>1.89</v>
+      </c>
+      <c r="F46" s="18"/>
+      <c r="G46" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H46" s="23">
+        <v>2.42</v>
+      </c>
+      <c r="I46" s="23">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A47" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="14">
+        <v>0.99</v>
+      </c>
+      <c r="D47" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="I47" s="22">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A48" s="18"/>
+      <c r="B48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="14">
+        <v>0.99</v>
+      </c>
+      <c r="D48" s="14">
+        <v>1</v>
+      </c>
+      <c r="F48" s="18"/>
+      <c r="G48" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="I48" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A49" s="18"/>
+      <c r="B49" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="15">
+        <v>0.98</v>
+      </c>
+      <c r="D49" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="F49" s="18"/>
+      <c r="G49" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H49" s="22">
+        <v>0.98</v>
+      </c>
+      <c r="I49" s="22">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A50" s="18"/>
+      <c r="B50" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="15">
+        <v>1</v>
+      </c>
+      <c r="D50" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="F50" s="18"/>
+      <c r="G50" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H50" s="22">
+        <v>1</v>
+      </c>
+      <c r="I50" s="22">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A51" s="18"/>
+      <c r="B51" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="15">
+        <v>2.04</v>
+      </c>
+      <c r="D51" s="15">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F51" s="18"/>
+      <c r="G51" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H51" s="22">
+        <v>2.04</v>
+      </c>
+      <c r="I51" s="22">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A52" s="18"/>
+      <c r="B52" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="16">
+        <v>5.67</v>
+      </c>
+      <c r="D52" s="16">
+        <v>3.82</v>
+      </c>
+      <c r="F52" s="18"/>
+      <c r="G52" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H52" s="23">
+        <v>5.67</v>
+      </c>
+      <c r="I52" s="23">
+        <v>3.82</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="F23:F28"/>
+    <mergeCell ref="F29:F34"/>
+    <mergeCell ref="F35:F40"/>
+    <mergeCell ref="F41:F46"/>
+    <mergeCell ref="F47:F52"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="F17:F22"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A41:A46"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0B0CB7-D6FF-45EF-AE95-0D14E70A71D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>